<commit_message>
Update version history and publish new excel sample
</commit_message>
<xml_diff>
--- a/DFW2Excel_Workbook_Example.xlsx
+++ b/DFW2Excel_Workbook_Example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10778" windowHeight="3330" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="9570" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Layer 3 Firewall" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="MACSETS" sheetId="4" r:id="rId6"/>
     <sheet name="Services" sheetId="3" r:id="rId7"/>
     <sheet name="Service Groups" sheetId="2" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="589">
   <si>
     <t>Service Group Configuration</t>
   </si>
@@ -1612,18 +1611,18 @@
     <t>VM Name</t>
   </si>
   <si>
+    <t>vm-70</t>
+  </si>
+  <si>
+    <t>vm1</t>
+  </si>
+  <si>
     <t>vm-103</t>
   </si>
   <si>
     <t>vm2</t>
   </si>
   <si>
-    <t>vm-70</t>
-  </si>
-  <si>
-    <t>vm1</t>
-  </si>
-  <si>
     <t>Security Tag Configuration</t>
   </si>
   <si>
@@ -1750,6 +1749,9 @@
     <t>any</t>
   </si>
   <si>
+    <t>NEGATE</t>
+  </si>
+  <si>
     <t>IPSet</t>
   </si>
   <si>
@@ -1768,13 +1770,13 @@
     <t>tonysangha.com</t>
   </si>
   <si>
+    <t>Cluster01</t>
+  </si>
+  <si>
     <t>deny</t>
   </si>
   <si>
     <t>ClusterComputeResource</t>
-  </si>
-  <si>
-    <t>Cluster01</t>
   </si>
   <si>
     <t xml:space="preserve"> Block Google DNS</t>
@@ -1845,14 +1847,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="52"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="52"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1899,8 +1901,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2181,32 +2183,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="22.5">
+    <row r="1" spans="1:17" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>547</v>
       </c>
@@ -2301,14 +2305,17 @@
       <c r="E4" s="2">
         <v>1008</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>572</v>
+      </c>
       <c r="G4" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H4" t="s">
         <v>507</v>
       </c>
       <c r="J4" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="K4" t="s">
         <v>505</v>
@@ -2326,7 +2333,7 @@
         <v>571</v>
       </c>
       <c r="P4" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="Q4" t="b">
         <v>1</v>
@@ -2337,19 +2344,19 @@
         <v>567</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="E5" s="2">
         <v>1007</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>575</v>
+      <c r="H5" s="8" t="s">
+        <v>576</v>
       </c>
       <c r="J5" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="K5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="L5" t="s">
         <v>15</v>
@@ -2364,7 +2371,7 @@
         <v>571</v>
       </c>
       <c r="P5" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="Q5" t="b">
         <v>0</v>
@@ -2376,27 +2383,27 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B9" s="2">
         <v>1004</v>
@@ -2408,25 +2415,19 @@
         <v>503</v>
       </c>
       <c r="E9" s="2">
-        <v>1006</v>
-      </c>
-      <c r="G9" t="s">
-        <v>572</v>
-      </c>
-      <c r="H9" t="s">
-        <v>507</v>
-      </c>
-      <c r="J9" t="s">
-        <v>572</v>
-      </c>
-      <c r="K9" t="s">
-        <v>505</v>
-      </c>
-      <c r="L9" t="s">
-        <v>202</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>578</v>
+        <v>1009</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>569</v>
       </c>
       <c r="N9" t="s">
         <v>570</v>
@@ -2435,228 +2436,272 @@
         <v>571</v>
       </c>
       <c r="P9" t="s">
+        <v>579</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="C10" t="s">
+        <v>567</v>
+      </c>
+      <c r="D10" t="s">
+        <v>503</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1006</v>
+      </c>
+      <c r="G10" t="s">
         <v>573</v>
       </c>
-      <c r="Q9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="H10" t="s">
+        <v>507</v>
+      </c>
       <c r="J10" t="s">
+        <v>573</v>
+      </c>
+      <c r="K10" t="s">
+        <v>505</v>
+      </c>
+      <c r="L10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="N10" t="s">
+        <v>570</v>
+      </c>
+      <c r="O10" t="s">
+        <v>571</v>
+      </c>
+      <c r="P10" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="J11" t="s">
+        <v>581</v>
+      </c>
+      <c r="K11" t="s">
         <v>579</v>
       </c>
-      <c r="K10" t="s">
+    </row>
+    <row r="12" spans="1:17">
+      <c r="C12" t="s">
+        <v>567</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1005</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="J12" t="s">
+        <v>583</v>
+      </c>
+      <c r="K12" t="s">
+        <v>584</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="7" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="C11" t="s">
+      <c r="N12" t="s">
+        <v>570</v>
+      </c>
+      <c r="O12" t="s">
+        <v>571</v>
+      </c>
+      <c r="P12" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="L13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1003</v>
+      </c>
+      <c r="C16" t="s">
         <v>567</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1005</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="J11" t="s">
-        <v>582</v>
-      </c>
-      <c r="K11" t="s">
-        <v>583</v>
-      </c>
-      <c r="L11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>578</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="D16" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1003</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="L16" t="s">
+        <v>264</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="N16" t="s">
         <v>570</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O16" t="s">
         <v>571</v>
       </c>
-      <c r="P11" t="s">
-        <v>573</v>
-      </c>
-      <c r="Q11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="L12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1003</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="P16" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="L17" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="C18" t="s">
         <v>567</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1003</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="L15" t="s">
-        <v>264</v>
-      </c>
-      <c r="M15" s="6" t="s">
+      <c r="D18" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1002</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="L18" t="s">
+        <v>207</v>
+      </c>
+      <c r="M18" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N18" t="s">
         <v>570</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O18" t="s">
         <v>571</v>
       </c>
-      <c r="P15" t="s">
-        <v>573</v>
-      </c>
-      <c r="Q15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="L16" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="C17" t="s">
+      <c r="P18" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="C20" t="s">
         <v>567</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1002</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="L17" t="s">
-        <v>207</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>569</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="D20" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1001</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="N20" t="s">
         <v>570</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O20" t="s">
         <v>571</v>
       </c>
-      <c r="P17" t="s">
-        <v>573</v>
-      </c>
-      <c r="Q17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="L18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="C19" t="s">
-        <v>567</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1001</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>578</v>
-      </c>
-      <c r="N19" t="s">
-        <v>570</v>
-      </c>
-      <c r="O19" t="s">
-        <v>571</v>
-      </c>
-      <c r="P19" t="s">
-        <v>573</v>
-      </c>
-      <c r="Q19" t="b">
+      <c r="P20" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q20" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
+    <row r="22" spans="1:17">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A8:Q8"/>
-    <mergeCell ref="A14:Q14"/>
-    <mergeCell ref="A21:Q21"/>
+    <mergeCell ref="A15:Q15"/>
+    <mergeCell ref="A22:Q22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2670,12 +2715,12 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>546</v>
       </c>
@@ -2692,12 +2737,12 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -2710,21 +2755,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>530</v>
       </c>
@@ -2756,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -2910,10 +2955,42 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>534</v>
+      </c>
+      <c r="B16" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>534</v>
+      </c>
+      <c r="B17" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>545</v>
+      </c>
+      <c r="B18" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -2932,20 +3009,20 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.5">
+    <row r="1" spans="1:10" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>509</v>
       </c>
@@ -3015,7 +3092,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="22.5">
+    <row r="4" spans="1:10" ht="23.25">
       <c r="A4" s="1" t="s">
         <v>522</v>
       </c>
@@ -3076,15 +3153,15 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.5">
+    <row r="1" spans="1:4" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>504</v>
       </c>
@@ -3150,14 +3227,14 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5">
+    <row r="1" spans="1:5" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>499</v>
       </c>
@@ -3200,20 +3277,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F416"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="83.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>240</v>
       </c>
@@ -10270,15 +10345,15 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5">
+    <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12613,16 +12688,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Object-ID for destination and source fields added to Layer 3 Firewall worksheet
</commit_message>
<xml_diff>
--- a/DFW2Excel_Workbook_Example.xlsx
+++ b/DFW2Excel_Workbook_Example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21555" windowHeight="9570" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10778" windowHeight="3330"/>
   </bookViews>
   <sheets>
     <sheet name="Layer 3 Firewall" sheetId="9" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="MACSETS" sheetId="4" r:id="rId6"/>
     <sheet name="Services" sheetId="3" r:id="rId7"/>
     <sheet name="Service Groups" sheetId="2" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="596">
   <si>
     <t>Service Group Configuration</t>
   </si>
@@ -1704,6 +1705,9 @@
     <t>Source Name</t>
   </si>
   <si>
+    <t>Source Object ID</t>
+  </si>
+  <si>
     <t>Destination Excluded (Negated)</t>
   </si>
   <si>
@@ -1713,6 +1717,9 @@
     <t>Destination Name</t>
   </si>
   <si>
+    <t>Destination Object ID</t>
+  </si>
+  <si>
     <t>Service Name</t>
   </si>
   <si>
@@ -1755,6 +1762,12 @@
     <t>IPSet</t>
   </si>
   <si>
+    <t>ipset-2</t>
+  </si>
+  <si>
+    <t>ipset-3</t>
+  </si>
+  <si>
     <t>DISTRIBUTED_FIREWALL</t>
   </si>
   <si>
@@ -1786,6 +1799,15 @@
   </si>
   <si>
     <t>8.8.8.8</t>
+  </si>
+  <si>
+    <t>Security Policy :: NSX Service Composer - Firewall</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
   <si>
     <t>Default Section Layer3</t>
@@ -2183,34 +2205,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.46484375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.25">
+    <row r="1" spans="1:19" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>547</v>
       </c>
@@ -2230,13 +2254,15 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="5" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>549</v>
       </c>
@@ -2288,101 +2314,116 @@
       <c r="Q3" s="3" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B4" s="2">
         <v>1005</v>
       </c>
       <c r="C4" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E4" s="2">
         <v>1008</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="G4" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="H4" t="s">
         <v>507</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" t="s">
+        <v>576</v>
+      </c>
+      <c r="K4" t="s">
+        <v>575</v>
+      </c>
+      <c r="L4" t="s">
+        <v>505</v>
+      </c>
+      <c r="M4" t="s">
+        <v>577</v>
+      </c>
+      <c r="N4" t="s">
+        <v>117</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="P4" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q4" t="s">
         <v>573</v>
       </c>
-      <c r="K4" t="s">
-        <v>505</v>
-      </c>
-      <c r="L4" t="s">
-        <v>117</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="R4" t="s">
+        <v>578</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="C5" t="s">
         <v>569</v>
       </c>
-      <c r="N4" t="s">
-        <v>570</v>
-      </c>
-      <c r="O4" t="s">
-        <v>571</v>
-      </c>
-      <c r="P4" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="C5" t="s">
-        <v>567</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="E5" s="2">
         <v>1007</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="J5" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="K5" t="s">
+        <v>581</v>
+      </c>
+      <c r="L5" t="s">
         <v>527</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
+        <v>526</v>
+      </c>
+      <c r="N5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>569</v>
-      </c>
-      <c r="N5" t="s">
-        <v>570</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="O5" s="6" t="s">
         <v>571</v>
       </c>
       <c r="P5" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="L6" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>573</v>
+      </c>
+      <c r="R5" t="s">
+        <v>578</v>
+      </c>
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="N6" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -2400,16 +2441,18 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="B9" s="2">
         <v>1004</v>
       </c>
       <c r="C9" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D9" t="s">
         <v>503</v>
@@ -2418,33 +2461,33 @@
         <v>1009</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="M9" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="P9" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>573</v>
+      </c>
+      <c r="R9" t="s">
+        <v>583</v>
+      </c>
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="C10" t="s">
         <v>569</v>
-      </c>
-      <c r="N9" t="s">
-        <v>570</v>
-      </c>
-      <c r="O9" t="s">
-        <v>571</v>
-      </c>
-      <c r="P9" t="s">
-        <v>579</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="C10" t="s">
-        <v>567</v>
       </c>
       <c r="D10" t="s">
         <v>503</v>
@@ -2453,91 +2496,100 @@
         <v>1006</v>
       </c>
       <c r="G10" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="H10" t="s">
         <v>507</v>
       </c>
-      <c r="J10" t="s">
+      <c r="I10" t="s">
+        <v>576</v>
+      </c>
+      <c r="K10" t="s">
+        <v>575</v>
+      </c>
+      <c r="L10" t="s">
+        <v>505</v>
+      </c>
+      <c r="M10" t="s">
+        <v>577</v>
+      </c>
+      <c r="N10" t="s">
+        <v>202</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="P10" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q10" t="s">
         <v>573</v>
       </c>
-      <c r="K10" t="s">
-        <v>505</v>
-      </c>
-      <c r="L10" t="s">
-        <v>202</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="N10" t="s">
-        <v>570</v>
-      </c>
-      <c r="O10" t="s">
-        <v>571</v>
-      </c>
-      <c r="P10" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="J11" t="s">
-        <v>581</v>
-      </c>
+      <c r="R10" t="s">
+        <v>578</v>
+      </c>
+      <c r="S10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="K11" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>585</v>
+      </c>
+      <c r="L11" t="s">
+        <v>583</v>
+      </c>
+      <c r="M11" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="C12" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="E12" s="2">
         <v>1005</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="I12" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="K12" t="s">
+        <v>587</v>
+      </c>
+      <c r="L12" t="s">
+        <v>588</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="P12" t="s">
         <v>572</v>
       </c>
-      <c r="J12" t="s">
-        <v>583</v>
-      </c>
-      <c r="K12" t="s">
-        <v>584</v>
-      </c>
-      <c r="L12" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="N12" t="s">
-        <v>570</v>
-      </c>
-      <c r="O12" t="s">
-        <v>571</v>
-      </c>
-      <c r="P12" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="L13" t="s">
+      <c r="Q12" t="s">
+        <v>573</v>
+      </c>
+      <c r="R12" t="s">
+        <v>578</v>
+      </c>
+      <c r="S12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="N13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:19">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -2555,153 +2607,220 @@
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="2" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="B16" s="2">
+        <v>1006</v>
+      </c>
+      <c r="C16" t="s">
+        <v>590</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1010</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="P16" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>573</v>
+      </c>
+      <c r="R16" t="s">
+        <v>578</v>
+      </c>
+      <c r="S16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B19" s="2">
         <v>1003</v>
       </c>
-      <c r="C16" t="s">
-        <v>567</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="C19" t="s">
+        <v>569</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="E19" s="2">
         <v>1003</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="H19" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="N19" t="s">
         <v>264</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="O19" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="P19" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>573</v>
+      </c>
+      <c r="R19" t="s">
+        <v>578</v>
+      </c>
+      <c r="S19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="N20" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="C21" t="s">
         <v>569</v>
       </c>
-      <c r="N16" t="s">
-        <v>570</v>
-      </c>
-      <c r="O16" t="s">
+      <c r="D21" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1002</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="N21" t="s">
+        <v>207</v>
+      </c>
+      <c r="O21" s="6" t="s">
         <v>571</v>
       </c>
-      <c r="P16" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="L17" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="C18" t="s">
-        <v>567</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1002</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="L18" t="s">
-        <v>207</v>
-      </c>
-      <c r="M18" s="6" t="s">
+      <c r="P21" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>573</v>
+      </c>
+      <c r="R21" t="s">
+        <v>578</v>
+      </c>
+      <c r="S21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="N22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="C23" t="s">
         <v>569</v>
       </c>
-      <c r="N18" t="s">
-        <v>570</v>
-      </c>
-      <c r="O18" t="s">
-        <v>571</v>
-      </c>
-      <c r="P18" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="L19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="C20" t="s">
-        <v>567</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D23" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="E23" s="2">
         <v>1001</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="M20" s="7" t="s">
+      <c r="H23" s="8" t="s">
         <v>580</v>
       </c>
-      <c r="N20" t="s">
-        <v>570</v>
-      </c>
-      <c r="O20" t="s">
-        <v>571</v>
-      </c>
-      <c r="P20" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q20" t="b">
+      <c r="M23" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="P23" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>573</v>
+      </c>
+      <c r="R23" t="s">
+        <v>578</v>
+      </c>
+      <c r="S23" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
+    <row r="25" spans="1:19">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A8:Q8"/>
-    <mergeCell ref="A15:Q15"/>
-    <mergeCell ref="A22:Q22"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A8:S8"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A18:S18"/>
+    <mergeCell ref="A25:S25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2715,12 +2834,12 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25">
+    <row r="1" spans="1:6" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>546</v>
       </c>
@@ -2761,15 +2880,15 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25">
+    <row r="1" spans="1:6" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>530</v>
       </c>
@@ -3009,20 +3128,20 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25">
+    <row r="1" spans="1:10" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>509</v>
       </c>
@@ -3092,7 +3211,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="23.25">
+    <row r="4" spans="1:10" ht="22.5">
       <c r="A4" s="1" t="s">
         <v>522</v>
       </c>
@@ -3153,15 +3272,15 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25">
+    <row r="1" spans="1:4" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>504</v>
       </c>
@@ -3227,14 +3346,14 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25">
+    <row r="1" spans="1:5" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>499</v>
       </c>
@@ -3277,18 +3396,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F416"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="94.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25">
+    <row r="1" spans="1:6" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>240</v>
       </c>
@@ -10341,19 +10462,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F389"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25">
+    <row r="1" spans="1:6" ht="22.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12686,6 +12807,18 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>